<commit_message>
Update academic session codes
</commit_message>
<xml_diff>
--- a/data/glossary/glossary_sgcm_academicsessioncode.xlsx
+++ b/data/glossary/glossary_sgcm_academicsessioncode.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce5345e3319cb7d5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dzulfaq\dtct2\data\glossary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8044CB34-BAD4-4BD5-9CB6-A5A4334D7FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3690BC-D1BA-475C-AC23-32B225CBED44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B923DCEC-98E6-40E1-8958-4BA113A2A895}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="930">
   <si>
     <t>Academic Session Code</t>
   </si>
@@ -2823,6 +2823,9 @@
   </si>
   <si>
     <t>TRIMESTER I 2025/2026 [F]</t>
+  </si>
+  <si>
+    <t>2026-02-3-FOUNDATION</t>
   </si>
 </sst>
 </file>
@@ -3224,10 +3227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DE4E58-099E-4000-9454-2B20039B69EE}">
-  <dimension ref="A1:B468"/>
+  <dimension ref="A1:B469"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A449" workbookViewId="0">
+      <selection activeCell="B465" sqref="B465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6980,6 +6983,14 @@
         <v>928</v>
       </c>
     </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A469">
+        <v>1</v>
+      </c>
+      <c r="B469" t="s">
+        <v>929</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>